<commit_message>
1.添加SensorBoard CMD设计草稿 2.增加ROMDriver模块，负责操作1-Wire EEPROM
</commit_message>
<xml_diff>
--- a/Doc/design/memory_layout.xlsx
+++ b/Doc/design/memory_layout.xlsx
@@ -322,6 +322,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -348,9 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -674,7 +674,7 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="3:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -685,29 +685,29 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C7" s="8"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="9"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -715,127 +715,127 @@
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C11" s="11"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C13" s="11"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C14" s="11"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C18" s="11"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C19" s="11"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C20" s="11"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C21" s="11"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C22" s="11"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C26" s="11"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C27" s="11"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C29" s="11"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C30" s="11"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.15">
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C33" s="11"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C34" s="11"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C35" s="11"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C36" s="11"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="11"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -846,25 +846,25 @@
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C41" s="11"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C42" s="11"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C43" s="11"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="11"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -875,11 +875,11 @@
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.15">
-      <c r="C46" s="14"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="15"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="5" t="s">
         <v>7</v>
       </c>
@@ -918,7 +918,7 @@
   <dimension ref="C1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -948,7 +948,7 @@
       </c>
     </row>
     <row r="6" spans="3:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>